<commit_message>
Update PAX reporting to accurately reflect individual ship data
Refactors the `ConsolidatedPaxProcessor` to introduce `generateSingleShipPax`. This new method bypasses aggregation and uses individual records to populate single-ship PAX reports, addressing discrepancies in sold figures.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a3af5c32-fe94-463b-bafd-8d7cf4140d74
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d67b414c-7ba7-46ed-90da-331e0aa9efb6/a3af5c32-fe94-463b-bafd-8d7cf4140d74/dpRBUiX
</commit_message>
<xml_diff>
--- a/output/ship-b/eod_1757351992206.xlsx
+++ b/output/ship-b/eod_1757351992206.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
   <si>
     <t>TOUR OPERATOR REPORT</t>
   </si>
@@ -1584,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q248"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C7" sqref="C7"/>
@@ -1887,7 +1887,7 @@
       <c r="H21" s="56"/>
     </row>
     <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" ht="36" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>31</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="G23" s="58"/>
       <c r="H23" s="59"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>33</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="62"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="60"/>
       <c r="B25" s="8"/>
       <c r="C25" s="63">
@@ -1935,7 +1935,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="62"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="60"/>
       <c r="B26" s="8"/>
       <c r="C26" s="63"/>
@@ -1945,7 +1945,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="62"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="64" t="s">
         <v>37</v>
       </c>
@@ -1957,7 +1957,7 @@
       <c r="G27" s="65"/>
       <c r="H27" s="66"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
         <v>38</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="G28" s="68"/>
       <c r="H28" s="69"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="70"/>
       <c r="B29" s="71"/>
       <c r="C29" s="71"/>
@@ -1979,7 +1979,7 @@
       <c r="G29" s="71"/>
       <c r="H29" s="72"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="70"/>
       <c r="B30" s="71"/>
       <c r="C30" s="71"/>
@@ -1989,7 +1989,7 @@
       <c r="G30" s="71"/>
       <c r="H30" s="72"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="70"/>
       <c r="B31" s="71"/>
       <c r="C31" s="71"/>
@@ -1999,7 +1999,7 @@
       <c r="G31" s="71"/>
       <c r="H31" s="72"/>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="70"/>
       <c r="B32" s="71"/>
       <c r="C32" s="71"/>
@@ -2009,7 +2009,7 @@
       <c r="G32" s="71"/>
       <c r="H32" s="72"/>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2023,7 +2023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
         <v>41</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="8"/>
       <c r="C35" s="61"/>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="H35" s="77"/>
     </row>
-    <row r="36" ht="15.6" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" ht="15.6" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="8"/>
       <c r="C36" s="61"/>
@@ -2061,7 +2061,7 @@
       <c r="G36" s="76"/>
       <c r="H36" s="78"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>33</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="G37" s="76"/>
       <c r="H37" s="79"/>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="80"/>
       <c r="B38" s="81"/>
       <c r="C38" s="82" t="s">
@@ -2099,6 +2099,7 @@
         <v>49</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="57" t="s">
         <v>31</v>
@@ -2140,7 +2141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
         <v>33</v>
       </c>
@@ -2158,7 +2159,7 @@
       <c r="G41" s="8"/>
       <c r="H41" s="62"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="8"/>
       <c r="C42" s="63">
@@ -2174,7 +2175,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="62"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="8"/>
       <c r="C43" s="63"/>
@@ -2184,7 +2185,7 @@
       <c r="G43" s="8"/>
       <c r="H43" s="62"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="86" t="s">
         <v>37</v>
       </c>
@@ -2196,7 +2197,7 @@
       <c r="G44" s="86"/>
       <c r="H44" s="86"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="87" t="s">
         <v>52</v>
       </c>
@@ -2208,7 +2209,7 @@
       <c r="G45" s="87"/>
       <c r="H45" s="87"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="87"/>
       <c r="B46" s="87"/>
       <c r="C46" s="87"/>
@@ -2218,7 +2219,7 @@
       <c r="G46" s="87"/>
       <c r="H46" s="87"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="87"/>
       <c r="B47" s="87"/>
       <c r="C47" s="87"/>
@@ -2228,7 +2229,7 @@
       <c r="G47" s="87"/>
       <c r="H47" s="87"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="87"/>
       <c r="B48" s="87"/>
       <c r="C48" s="87"/>
@@ -2238,7 +2239,7 @@
       <c r="G48" s="87"/>
       <c r="H48" s="87"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="87"/>
       <c r="B49" s="87"/>
       <c r="C49" s="87"/>
@@ -2248,7 +2249,7 @@
       <c r="G49" s="87"/>
       <c r="H49" s="87"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="60"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -2262,7 +2263,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="60" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="60"/>
       <c r="B52" s="8"/>
       <c r="C52" s="61"/>
@@ -2290,7 +2291,7 @@
       </c>
       <c r="H52" s="77"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="60"/>
       <c r="B53" s="8"/>
       <c r="C53" s="61"/>
@@ -2300,7 +2301,7 @@
       <c r="G53" s="76"/>
       <c r="H53" s="78"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="60" t="s">
         <v>33</v>
       </c>
@@ -2318,7 +2319,7 @@
       <c r="G54" s="76"/>
       <c r="H54" s="79"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="80"/>
       <c r="B55" s="81"/>
       <c r="C55" s="82" t="s">
@@ -2338,7 +2339,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="57" t="s">
         <v>31</v>
@@ -2380,7 +2381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="60" t="s">
         <v>33</v>
       </c>
@@ -2398,7 +2399,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="62"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
       <c r="B59" s="8"/>
       <c r="C59" s="63">
@@ -2414,7 +2415,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="62"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="60"/>
       <c r="B60" s="8"/>
       <c r="C60" s="63"/>
@@ -2424,7 +2425,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="62"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="86" t="s">
         <v>37</v>
       </c>
@@ -2436,7 +2437,7 @@
       <c r="G61" s="86"/>
       <c r="H61" s="86"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="87" t="s">
         <v>38</v>
       </c>
@@ -2448,7 +2449,7 @@
       <c r="G62" s="87"/>
       <c r="H62" s="87"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="87"/>
       <c r="B63" s="87"/>
       <c r="C63" s="87"/>
@@ -2458,7 +2459,7 @@
       <c r="G63" s="87"/>
       <c r="H63" s="87"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="87"/>
       <c r="B64" s="87"/>
       <c r="C64" s="87"/>
@@ -2468,7 +2469,7 @@
       <c r="G64" s="87"/>
       <c r="H64" s="87"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="87"/>
       <c r="B65" s="87"/>
       <c r="C65" s="87"/>
@@ -2478,7 +2479,7 @@
       <c r="G65" s="87"/>
       <c r="H65" s="87"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="87"/>
       <c r="B66" s="87"/>
       <c r="C66" s="87"/>
@@ -2488,7 +2489,7 @@
       <c r="G66" s="87"/>
       <c r="H66" s="87"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="60"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -2502,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="60" t="s">
         <v>41</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="60"/>
       <c r="B69" s="8"/>
       <c r="C69" s="61"/>
@@ -2530,7 +2531,7 @@
       </c>
       <c r="H69" s="77"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="60"/>
       <c r="B70" s="8"/>
       <c r="C70" s="61"/>
@@ -2540,7 +2541,7 @@
       <c r="G70" s="76"/>
       <c r="H70" s="78"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="60" t="s">
         <v>33</v>
       </c>
@@ -2558,7 +2559,7 @@
       <c r="G71" s="76"/>
       <c r="H71" s="79"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="80"/>
       <c r="B72" s="81"/>
       <c r="C72" s="82" t="s">
@@ -2578,8 +2579,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="88" t="s">
         <v>54</v>
       </c>
@@ -2591,7 +2592,7 @@
       <c r="G74" s="89"/>
       <c r="H74" s="89"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="92"/>
       <c r="B75" s="92"/>
       <c r="C75" s="92"/>
@@ -2601,7 +2602,7 @@
       <c r="G75" s="92"/>
       <c r="H75" s="92"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="93"/>
       <c r="B76" s="89"/>
       <c r="C76" s="61" t="s">
@@ -2617,7 +2618,7 @@
       <c r="G76" s="89"/>
       <c r="H76" s="89"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="94" t="s">
         <v>55</v>
       </c>
@@ -2637,10 +2638,767 @@
       <c r="G77" s="95"/>
       <c r="H77" s="95"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="85"/>
+      <c r="D83" s="85"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="85"/>
+      <c r="H83" s="85"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="62"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="60"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="63">
+        <v>49</v>
+      </c>
+      <c r="D85" s="63">
+        <v>5</v>
+      </c>
+      <c r="E85" s="63">
+        <v>1</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="62"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="60"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="63"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="62"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" s="86"/>
+      <c r="C87" s="86"/>
+      <c r="D87" s="86"/>
+      <c r="E87" s="86"/>
+      <c r="F87" s="86"/>
+      <c r="G87" s="86"/>
+      <c r="H87" s="86"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="87"/>
+      <c r="C88" s="87"/>
+      <c r="D88" s="87"/>
+      <c r="E88" s="87"/>
+      <c r="F88" s="87"/>
+      <c r="G88" s="87"/>
+      <c r="H88" s="87"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="87"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="87"/>
+      <c r="D89" s="87"/>
+      <c r="E89" s="87"/>
+      <c r="F89" s="87"/>
+      <c r="G89" s="87"/>
+      <c r="H89" s="87"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="87"/>
+      <c r="B90" s="87"/>
+      <c r="C90" s="87"/>
+      <c r="D90" s="87"/>
+      <c r="E90" s="87"/>
+      <c r="F90" s="87"/>
+      <c r="G90" s="87"/>
+      <c r="H90" s="87"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="87"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="87"/>
+      <c r="D91" s="87"/>
+      <c r="E91" s="87"/>
+      <c r="F91" s="87"/>
+      <c r="G91" s="87"/>
+      <c r="H91" s="87"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="87"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="87"/>
+      <c r="D92" s="87"/>
+      <c r="E92" s="87"/>
+      <c r="F92" s="87"/>
+      <c r="G92" s="87"/>
+      <c r="H92" s="87"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="60"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H93" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="75"/>
+      <c r="G94" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H94" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="60"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="61"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="61"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H95" s="77"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="60"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="61"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="61"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="78"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E97" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="79"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="80"/>
+      <c r="B98" s="81"/>
+      <c r="C98" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D98" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F98" s="81"/>
+      <c r="G98" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H98" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B99" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" s="85"/>
+      <c r="D99" s="85"/>
+      <c r="E99" s="85"/>
+      <c r="F99" s="85"/>
+      <c r="G99" s="85"/>
+      <c r="H99" s="85"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D100" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E100" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="62"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="60"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="63">
+        <v>52</v>
+      </c>
+      <c r="D101" s="63">
+        <v>2</v>
+      </c>
+      <c r="E101" s="63">
+        <v>1</v>
+      </c>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="62"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="60"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="62"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B103" s="86"/>
+      <c r="C103" s="86"/>
+      <c r="D103" s="86"/>
+      <c r="E103" s="86"/>
+      <c r="F103" s="86"/>
+      <c r="G103" s="86"/>
+      <c r="H103" s="86"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B104" s="87"/>
+      <c r="C104" s="87"/>
+      <c r="D104" s="87"/>
+      <c r="E104" s="87"/>
+      <c r="F104" s="87"/>
+      <c r="G104" s="87"/>
+      <c r="H104" s="87"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="87"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="87"/>
+      <c r="D105" s="87"/>
+      <c r="E105" s="87"/>
+      <c r="F105" s="87"/>
+      <c r="G105" s="87"/>
+      <c r="H105" s="87"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="87"/>
+      <c r="B106" s="87"/>
+      <c r="C106" s="87"/>
+      <c r="D106" s="87"/>
+      <c r="E106" s="87"/>
+      <c r="F106" s="87"/>
+      <c r="G106" s="87"/>
+      <c r="H106" s="87"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="87"/>
+      <c r="B107" s="87"/>
+      <c r="C107" s="87"/>
+      <c r="D107" s="87"/>
+      <c r="E107" s="87"/>
+      <c r="F107" s="87"/>
+      <c r="G107" s="87"/>
+      <c r="H107" s="87"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="87"/>
+      <c r="B108" s="87"/>
+      <c r="C108" s="87"/>
+      <c r="D108" s="87"/>
+      <c r="E108" s="87"/>
+      <c r="F108" s="87"/>
+      <c r="G108" s="87"/>
+      <c r="H108" s="87"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="60"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H109" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="75"/>
+      <c r="G110" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H110" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="60"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="61"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="61"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H111" s="77"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="60"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="61"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="61"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="76"/>
+      <c r="H112" s="78"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D113" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E113" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F113" s="8"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="79"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="80"/>
+      <c r="B114" s="81"/>
+      <c r="C114" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D114" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F114" s="81"/>
+      <c r="G114" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H114" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" s="85"/>
+      <c r="D115" s="85"/>
+      <c r="E115" s="85"/>
+      <c r="F115" s="85"/>
+      <c r="G115" s="85"/>
+      <c r="H115" s="85"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" s="8"/>
+      <c r="C116" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D116" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E116" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="62"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="60"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="63">
+        <v>47</v>
+      </c>
+      <c r="D117" s="63">
+        <v>3</v>
+      </c>
+      <c r="E117" s="63">
+        <v>0</v>
+      </c>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="62"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="60"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="63"/>
+      <c r="D118" s="63"/>
+      <c r="E118" s="63"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="62"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B119" s="86"/>
+      <c r="C119" s="86"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
+      <c r="G119" s="86"/>
+      <c r="H119" s="86"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" s="87"/>
+      <c r="C120" s="87"/>
+      <c r="D120" s="87"/>
+      <c r="E120" s="87"/>
+      <c r="F120" s="87"/>
+      <c r="G120" s="87"/>
+      <c r="H120" s="87"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="87"/>
+      <c r="B121" s="87"/>
+      <c r="C121" s="87"/>
+      <c r="D121" s="87"/>
+      <c r="E121" s="87"/>
+      <c r="F121" s="87"/>
+      <c r="G121" s="87"/>
+      <c r="H121" s="87"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="87"/>
+      <c r="B122" s="87"/>
+      <c r="C122" s="87"/>
+      <c r="D122" s="87"/>
+      <c r="E122" s="87"/>
+      <c r="F122" s="87"/>
+      <c r="G122" s="87"/>
+      <c r="H122" s="87"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="87"/>
+      <c r="B123" s="87"/>
+      <c r="C123" s="87"/>
+      <c r="D123" s="87"/>
+      <c r="E123" s="87"/>
+      <c r="F123" s="87"/>
+      <c r="G123" s="87"/>
+      <c r="H123" s="87"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="87"/>
+      <c r="B124" s="87"/>
+      <c r="C124" s="87"/>
+      <c r="D124" s="87"/>
+      <c r="E124" s="87"/>
+      <c r="F124" s="87"/>
+      <c r="G124" s="87"/>
+      <c r="H124" s="87"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="60"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="8"/>
+      <c r="G125" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H125" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B126" s="8"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="75"/>
+      <c r="G126" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H126" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="60"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H127" s="77"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="60"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="76"/>
+      <c r="H128" s="78"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B129" s="8"/>
+      <c r="C129" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D129" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E129" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="8"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="79"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="80"/>
+      <c r="B130" s="81"/>
+      <c r="C130" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D130" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E130" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F130" s="81"/>
+      <c r="G130" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H130" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="33">
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
@@ -2665,6 +3423,15 @@
     <mergeCell ref="A61:H61"/>
     <mergeCell ref="A62:H66"/>
     <mergeCell ref="C68:F68"/>
+    <mergeCell ref="B83:H83"/>
+    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A88:H92"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="A103:H103"/>
+    <mergeCell ref="A104:H108"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="A120:H124"/>
   </mergeCells>
   <conditionalFormatting sqref="A28">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">

</xml_diff>